<commit_message>
run everything again and add clinvar data to the main folder
</commit_message>
<xml_diff>
--- a/fisher_for_all_data.xlsx
+++ b/fisher_for_all_data.xlsx
@@ -588,31 +588,31 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Scoliosis</t>
+          <t>Alzheimer's Disease</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CNCCs</t>
+          <t>Cortical_organoids_d100</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.608940531763751</v>
+        <v>0.6683710831609646</v>
       </c>
       <c r="D3" t="n">
-        <v>1.989960515490272e-05</v>
+        <v>2.195838542923922e-05</v>
       </c>
       <c r="E3" t="n">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="F3" t="n">
-        <v>208</v>
+        <v>562</v>
       </c>
       <c r="G3" t="n">
-        <v>3411</v>
+        <v>2770</v>
       </c>
       <c r="H3" t="n">
-        <v>7713</v>
+        <v>7432</v>
       </c>
       <c r="I3" t="n">
         <v>0.000395250937726306</v>
@@ -621,25 +621,25 @@
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>1.082601054481547</v>
+        <v>1.12472487160675</v>
       </c>
       <c r="L3" t="n">
-        <v>0.6749014804308221</v>
+        <v>0.5444108617705408</v>
       </c>
       <c r="M3" t="n">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="N3" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="O3" t="n">
-        <v>1707</v>
+        <v>1363</v>
       </c>
       <c r="P3" t="n">
-        <v>1704</v>
+        <v>1407</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.9503205265004374</v>
+        <v>0.928944418095249</v>
       </c>
       <c r="R3" t="b">
         <v>0</v>
@@ -648,31 +648,31 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Alzheimer's Disease</t>
+          <t>Scoliosis</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cortical_organoids_d100</t>
+          <t>CNCCs</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.6683710831609646</v>
+        <v>1.608940531763751</v>
       </c>
       <c r="D4" t="n">
-        <v>2.195838542923922e-05</v>
+        <v>1.989960515490272e-05</v>
       </c>
       <c r="E4" t="n">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="F4" t="n">
-        <v>562</v>
+        <v>208</v>
       </c>
       <c r="G4" t="n">
-        <v>2770</v>
+        <v>3411</v>
       </c>
       <c r="H4" t="n">
-        <v>7432</v>
+        <v>7713</v>
       </c>
       <c r="I4" t="n">
         <v>0.000395250937726306</v>
@@ -681,25 +681,25 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>1.12472487160675</v>
+        <v>1.082601054481547</v>
       </c>
       <c r="L4" t="n">
-        <v>0.5444108617705408</v>
+        <v>0.6749014804308221</v>
       </c>
       <c r="M4" t="n">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="N4" t="n">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="O4" t="n">
-        <v>1363</v>
+        <v>1707</v>
       </c>
       <c r="P4" t="n">
-        <v>1407</v>
+        <v>1704</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.928944418095249</v>
+        <v>0.9503205265004374</v>
       </c>
       <c r="R4" t="b">
         <v>0</v>
@@ -1008,31 +1008,31 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ovarian polycystic syndrome (PCOS)</t>
+          <t>Back Disorders</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Cortical_organoids_d50</t>
+          <t>4_Prechondral_Mesenchyme</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.1773528847996933</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.07437721465595361</v>
+        <v>0.07907646134494326</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="G10" t="n">
-        <v>3478</v>
+        <v>386</v>
       </c>
       <c r="H10" t="n">
-        <v>7402</v>
+        <v>9300</v>
       </c>
       <c r="I10" t="n">
         <v>0.40297249592384</v>
@@ -1112,31 +1112,31 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Back Disorders</t>
+          <t>Ovarian polycystic syndrome (PCOS)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4_Prechondral_Mesenchyme</t>
+          <t>Cortical_organoids_d50</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>0.1773528847996933</v>
       </c>
       <c r="D12" t="n">
-        <v>0.07907646134494326</v>
+        <v>0.07437721465595361</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G12" t="n">
-        <v>386</v>
+        <v>3478</v>
       </c>
       <c r="H12" t="n">
-        <v>9300</v>
+        <v>7402</v>
       </c>
       <c r="I12" t="n">
         <v>0.40297249592384</v>
@@ -1380,31 +1380,31 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Varicose veins</t>
+          <t>Colon diverticulosis</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Endothelial_not_treated</t>
+          <t>Skeletal_myocyte_(SKM)</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.3048483598101919</v>
+        <v>1.463838487094301</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1416314841859758</v>
+        <v>0.1470466708278776</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F17" t="n">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="G17" t="n">
-        <v>4847</v>
+        <v>3010</v>
       </c>
       <c r="H17" t="n">
-        <v>7388</v>
+        <v>11456</v>
       </c>
       <c r="I17" t="n">
         <v>0.4670894249826701</v>
@@ -1412,43 +1412,59 @@
       <c r="J17" t="b">
         <v>0</v>
       </c>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
+      <c r="K17" t="n">
+        <v>0.8236363636363636</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.8232465332793673</v>
+      </c>
+      <c r="M17" t="n">
+        <v>9</v>
+      </c>
+      <c r="N17" t="n">
+        <v>11</v>
+      </c>
+      <c r="O17" t="n">
+        <v>1500</v>
+      </c>
+      <c r="P17" t="n">
+        <v>1510</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.9503205265004374</v>
+      </c>
+      <c r="R17" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Colon diverticulosis</t>
+          <t>Varicose veins</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Skeletal_myocyte_(SKM)</t>
+          <t>Endothelial_not_treated</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1.463838487094301</v>
+        <v>0.3048483598101919</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1470466708278776</v>
+        <v>0.1416314841859758</v>
       </c>
       <c r="E18" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="G18" t="n">
-        <v>3010</v>
+        <v>4847</v>
       </c>
       <c r="H18" t="n">
-        <v>11456</v>
+        <v>7388</v>
       </c>
       <c r="I18" t="n">
         <v>0.4670894249826701</v>
@@ -1456,59 +1472,43 @@
       <c r="J18" t="b">
         <v>0</v>
       </c>
-      <c r="K18" t="n">
-        <v>0.8236363636363636</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0.8232465332793673</v>
-      </c>
-      <c r="M18" t="n">
-        <v>9</v>
-      </c>
-      <c r="N18" t="n">
-        <v>11</v>
-      </c>
-      <c r="O18" t="n">
-        <v>1500</v>
-      </c>
-      <c r="P18" t="n">
-        <v>1510</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>0.9503205265004374</v>
-      </c>
-      <c r="R18" t="b">
-        <v>0</v>
-      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>carcinoma</t>
+          <t>Bipolar disorder</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Pooled_epidermis</t>
+          <t>Cortical_organoids_d100</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.7342389374245329</v>
+        <v>0.8306901905434015</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1771624268749524</v>
+        <v>0.181724572324664</v>
       </c>
       <c r="E19" t="n">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="F19" t="n">
-        <v>741</v>
+        <v>250</v>
       </c>
       <c r="G19" t="n">
-        <v>380</v>
+        <v>2834</v>
       </c>
       <c r="H19" t="n">
-        <v>8989</v>
+        <v>7744</v>
       </c>
       <c r="I19" t="n">
         <v>0.4672917574062788</v>
@@ -1517,22 +1517,22 @@
         <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>2.486656200941915</v>
+        <v>0.6257920125814695</v>
       </c>
       <c r="L19" t="n">
-        <v>0.0531601843025519</v>
+        <v>0.04894373111450499</v>
       </c>
       <c r="M19" t="n">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="N19" t="n">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="O19" t="n">
-        <v>182</v>
+        <v>1407</v>
       </c>
       <c r="P19" t="n">
-        <v>198</v>
+        <v>1427</v>
       </c>
       <c r="Q19" t="n">
         <v>0.3189611058153114</v>
@@ -1544,31 +1544,31 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Hemorrhoids</t>
+          <t>Osteoarthritis</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Pooled_fibroblasts</t>
+          <t>4_Prechondral_Mesenchyme</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.2303715141306382</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1790880746267531</v>
+        <v>0.1759116570297418</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="G20" t="n">
-        <v>1096</v>
+        <v>386</v>
       </c>
       <c r="H20" t="n">
-        <v>9847</v>
+        <v>9322</v>
       </c>
       <c r="I20" t="n">
         <v>0.4672917574062788</v>
@@ -1588,31 +1588,31 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Osteoarthritis</t>
+          <t>carcinoma</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4_Prechondral_Mesenchyme</t>
+          <t>Pooled_epidermis</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>0.7342389374245329</v>
       </c>
       <c r="D21" t="n">
-        <v>0.1759116570297418</v>
+        <v>0.1771624268749524</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F21" t="n">
-        <v>60</v>
+        <v>741</v>
       </c>
       <c r="G21" t="n">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="H21" t="n">
-        <v>9322</v>
+        <v>8989</v>
       </c>
       <c r="I21" t="n">
         <v>0.4672917574062788</v>
@@ -1620,43 +1620,59 @@
       <c r="J21" t="b">
         <v>0</v>
       </c>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr"/>
+      <c r="K21" t="n">
+        <v>2.486656200941915</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.0531601843025519</v>
+      </c>
+      <c r="M21" t="n">
+        <v>16</v>
+      </c>
+      <c r="N21" t="n">
+        <v>7</v>
+      </c>
+      <c r="O21" t="n">
+        <v>182</v>
+      </c>
+      <c r="P21" t="n">
+        <v>198</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.3189611058153114</v>
+      </c>
+      <c r="R21" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Bipolar disorder</t>
+          <t>Hemorrhoids</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Cortical_organoids_d100</t>
+          <t>Pooled_fibroblasts</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.8306901905434015</v>
+        <v>0.2303715141306382</v>
       </c>
       <c r="D22" t="n">
-        <v>0.181724572324664</v>
+        <v>0.1790880746267531</v>
       </c>
       <c r="E22" t="n">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>250</v>
+        <v>39</v>
       </c>
       <c r="G22" t="n">
-        <v>2834</v>
+        <v>1096</v>
       </c>
       <c r="H22" t="n">
-        <v>7744</v>
+        <v>9847</v>
       </c>
       <c r="I22" t="n">
         <v>0.4672917574062788</v>
@@ -1664,30 +1680,14 @@
       <c r="J22" t="b">
         <v>0</v>
       </c>
-      <c r="K22" t="n">
-        <v>0.6257920125814695</v>
-      </c>
-      <c r="L22" t="n">
-        <v>0.04894373111450499</v>
-      </c>
-      <c r="M22" t="n">
-        <v>29</v>
-      </c>
-      <c r="N22" t="n">
-        <v>47</v>
-      </c>
-      <c r="O22" t="n">
-        <v>1407</v>
-      </c>
-      <c r="P22" t="n">
-        <v>1427</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>0.3189611058153114</v>
-      </c>
-      <c r="R22" t="b">
-        <v>0</v>
-      </c>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2344,31 +2344,31 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>premature birth</t>
+          <t>Bronchial asthma</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>iPSCs</t>
+          <t>Pooled_epidermis</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1.172855907344169</v>
+        <v>0.7808171246269425</v>
       </c>
       <c r="D36" t="n">
-        <v>0.6377655692143989</v>
+        <v>0.6251472040828558</v>
       </c>
       <c r="E36" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F36" t="n">
-        <v>19</v>
+        <v>246</v>
       </c>
       <c r="G36" t="n">
-        <v>5903</v>
+        <v>395</v>
       </c>
       <c r="H36" t="n">
-        <v>6264</v>
+        <v>9484</v>
       </c>
       <c r="I36" t="n">
         <v>0.9566483538215983</v>
@@ -2376,59 +2376,43 @@
       <c r="J36" t="b">
         <v>0</v>
       </c>
-      <c r="K36" t="n">
-        <v>1.098138117806364</v>
-      </c>
-      <c r="L36" t="n">
-        <v>1</v>
-      </c>
-      <c r="M36" t="n">
-        <v>11</v>
-      </c>
-      <c r="N36" t="n">
-        <v>10</v>
-      </c>
-      <c r="O36" t="n">
-        <v>2954</v>
-      </c>
-      <c r="P36" t="n">
-        <v>2949</v>
-      </c>
-      <c r="Q36" t="n">
-        <v>1</v>
-      </c>
-      <c r="R36" t="b">
-        <v>0</v>
-      </c>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr"/>
+      <c r="R36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Bronchial asthma</t>
+          <t>premature birth</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Pooled_epidermis</t>
+          <t>iPSCs</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.7808171246269425</v>
+        <v>1.172855907344169</v>
       </c>
       <c r="D37" t="n">
-        <v>0.6251472040828558</v>
+        <v>0.6377655692143989</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F37" t="n">
-        <v>246</v>
+        <v>19</v>
       </c>
       <c r="G37" t="n">
-        <v>395</v>
+        <v>5903</v>
       </c>
       <c r="H37" t="n">
-        <v>9484</v>
+        <v>6264</v>
       </c>
       <c r="I37" t="n">
         <v>0.9566483538215983</v>
@@ -2436,14 +2420,30 @@
       <c r="J37" t="b">
         <v>0</v>
       </c>
-      <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr"/>
-      <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr"/>
-      <c r="P37" t="inlineStr"/>
-      <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr"/>
+      <c r="K37" t="n">
+        <v>1.098138117806364</v>
+      </c>
+      <c r="L37" t="n">
+        <v>1</v>
+      </c>
+      <c r="M37" t="n">
+        <v>11</v>
+      </c>
+      <c r="N37" t="n">
+        <v>10</v>
+      </c>
+      <c r="O37" t="n">
+        <v>2954</v>
+      </c>
+      <c r="P37" t="n">
+        <v>2949</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>1</v>
+      </c>
+      <c r="R37" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2508,31 +2508,31 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Bronchial asthma</t>
+          <t>Scoliosis</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Skeletal_myocyte_(SKM)</t>
+          <t>9_Chondrocytes</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.9583581507957776</v>
+        <v>0.6099667774086379</v>
       </c>
       <c r="D39" t="n">
-        <v>0.7933947164465431</v>
+        <v>0.7730263349053912</v>
       </c>
       <c r="E39" t="n">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
-        <v>289</v>
+        <v>215</v>
       </c>
       <c r="G39" t="n">
-        <v>2957</v>
+        <v>105</v>
       </c>
       <c r="H39" t="n">
-        <v>11219</v>
+        <v>6885</v>
       </c>
       <c r="I39" t="n">
         <v>1</v>
@@ -2540,35 +2540,19 @@
       <c r="J39" t="b">
         <v>0</v>
       </c>
-      <c r="K39" t="n">
-        <v>1.096785471496552</v>
-      </c>
-      <c r="L39" t="n">
-        <v>0.723448293904273</v>
-      </c>
-      <c r="M39" t="n">
-        <v>38</v>
-      </c>
-      <c r="N39" t="n">
-        <v>35</v>
-      </c>
-      <c r="O39" t="n">
-        <v>1471</v>
-      </c>
-      <c r="P39" t="n">
-        <v>1486</v>
-      </c>
-      <c r="Q39" t="n">
-        <v>0.9503205265004374</v>
-      </c>
-      <c r="R39" t="b">
-        <v>0</v>
-      </c>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr"/>
+      <c r="R39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Osteoarthritis</t>
+          <t>Back Disorders</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2586,13 +2570,13 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G40" t="n">
         <v>76</v>
       </c>
       <c r="H40" t="n">
-        <v>6948</v>
+        <v>6945</v>
       </c>
       <c r="I40" t="n">
         <v>1</v>
@@ -2612,31 +2596,31 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Sleep apnea</t>
+          <t>carcinoma</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Cortical_organoids_d100</t>
+          <t>Hepatocyte_Progenitor_(HP)</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.9156060084852654</v>
+        <v>0.9987109652706972</v>
       </c>
       <c r="D41" t="n">
         <v>1</v>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>438</v>
       </c>
       <c r="F41" t="n">
-        <v>9</v>
+        <v>568</v>
       </c>
       <c r="G41" t="n">
-        <v>2907</v>
+        <v>5567</v>
       </c>
       <c r="H41" t="n">
-        <v>7985</v>
+        <v>7210</v>
       </c>
       <c r="I41" t="n">
         <v>1</v>
@@ -2644,43 +2628,59 @@
       <c r="J41" t="b">
         <v>0</v>
       </c>
-      <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr"/>
-      <c r="N41" t="inlineStr"/>
-      <c r="O41" t="inlineStr"/>
-      <c r="P41" t="inlineStr"/>
-      <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr"/>
+      <c r="K41" t="n">
+        <v>1.073898606097515</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0.4873909825454742</v>
+      </c>
+      <c r="M41" t="n">
+        <v>227</v>
+      </c>
+      <c r="N41" t="n">
+        <v>211</v>
+      </c>
+      <c r="O41" t="n">
+        <v>2786</v>
+      </c>
+      <c r="P41" t="n">
+        <v>2781</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0.928944418095249</v>
+      </c>
+      <c r="R41" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Back Disorders</t>
+          <t>Colon diverticulosis</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>8_Also_Prechondral_Mesenchyme</t>
+          <t>Pooled_epidermis</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>0.985393658710367</v>
       </c>
       <c r="D42" t="n">
         <v>1</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G42" t="n">
-        <v>76</v>
+        <v>401</v>
       </c>
       <c r="H42" t="n">
-        <v>6945</v>
+        <v>9681</v>
       </c>
       <c r="I42" t="n">
         <v>1</v>
@@ -2700,31 +2700,31 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Sleep apnea</t>
+          <t>Acne vulgaris</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Cortical_organoids_d50</t>
+          <t>HF_Sebocytes</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.7101074031453778</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>0.7626901108875515</v>
+        <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G43" t="n">
-        <v>3476</v>
+        <v>70</v>
       </c>
       <c r="H43" t="n">
-        <v>7405</v>
+        <v>5404</v>
       </c>
       <c r="I43" t="n">
         <v>1</v>
@@ -2744,31 +2744,31 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Sleep apnea</t>
+          <t>Acne vulgaris</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Skeletal_myocyte_(SKM)</t>
+          <t>Keratinocytes</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.9494549058473737</v>
+        <v>1.032620320855615</v>
       </c>
       <c r="D44" t="n">
         <v>1</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G44" t="n">
-        <v>3027</v>
+        <v>850</v>
       </c>
       <c r="H44" t="n">
-        <v>11496</v>
+        <v>9655</v>
       </c>
       <c r="I44" t="n">
         <v>1</v>
@@ -2788,31 +2788,31 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Ovarian polycystic syndrome (PCOS)</t>
+          <t>Acne vulgaris</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Cortical_organoids_d100</t>
+          <t>Pooled_fibroblasts</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.7489445538981143</v>
+        <v>0.8580126114372689</v>
       </c>
       <c r="D45" t="n">
-        <v>0.7721074750517859</v>
+        <v>1</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G45" t="n">
-        <v>2907</v>
+        <v>1095</v>
       </c>
       <c r="H45" t="n">
-        <v>7983</v>
+        <v>9865</v>
       </c>
       <c r="I45" t="n">
         <v>1</v>
@@ -2832,31 +2832,31 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>aneurysm</t>
+          <t>Sleep apnea</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Pooled_fibroblasts</t>
+          <t>Cortical_organoids_d50</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1.092683467797832</v>
+        <v>0.7101074031453778</v>
       </c>
       <c r="D46" t="n">
-        <v>0.7834449794144795</v>
+        <v>0.7626901108875515</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="G46" t="n">
-        <v>1093</v>
+        <v>3476</v>
       </c>
       <c r="H46" t="n">
-        <v>9853</v>
+        <v>7405</v>
       </c>
       <c r="I46" t="n">
         <v>1</v>
@@ -2876,31 +2876,31 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>carcinoma</t>
+          <t>Sleep apnea</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Hepatocyte_Progenitor_(HP)</t>
+          <t>Skeletal_myocyte_(SKM)</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.9987109652706972</v>
+        <v>0.9494549058473737</v>
       </c>
       <c r="D47" t="n">
         <v>1</v>
       </c>
       <c r="E47" t="n">
-        <v>438</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
-        <v>568</v>
+        <v>12</v>
       </c>
       <c r="G47" t="n">
-        <v>5567</v>
+        <v>3027</v>
       </c>
       <c r="H47" t="n">
-        <v>7210</v>
+        <v>11496</v>
       </c>
       <c r="I47" t="n">
         <v>1</v>
@@ -2908,35 +2908,19 @@
       <c r="J47" t="b">
         <v>0</v>
       </c>
-      <c r="K47" t="n">
-        <v>1.073898606097515</v>
-      </c>
-      <c r="L47" t="n">
-        <v>0.4873909825454742</v>
-      </c>
-      <c r="M47" t="n">
-        <v>227</v>
-      </c>
-      <c r="N47" t="n">
-        <v>211</v>
-      </c>
-      <c r="O47" t="n">
-        <v>2786</v>
-      </c>
-      <c r="P47" t="n">
-        <v>2781</v>
-      </c>
-      <c r="Q47" t="n">
-        <v>0.928944418095249</v>
-      </c>
-      <c r="R47" t="b">
-        <v>0</v>
-      </c>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr"/>
+      <c r="R47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Acne vulgaris</t>
+          <t>Psoriasis</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2945,22 +2929,22 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1.032620320855615</v>
+        <v>1.082292018462231</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>0.8234780967067024</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="G48" t="n">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="H48" t="n">
-        <v>9655</v>
+        <v>9614</v>
       </c>
       <c r="I48" t="n">
         <v>1</v>
@@ -2980,31 +2964,31 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Acne vulgaris</t>
+          <t>Sleep apnea</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Pooled_fibroblasts</t>
+          <t>Cortical_organoids_d100</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.8580126114372689</v>
+        <v>0.9156060084852654</v>
       </c>
       <c r="D49" t="n">
         <v>1</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G49" t="n">
-        <v>1095</v>
+        <v>2907</v>
       </c>
       <c r="H49" t="n">
-        <v>9865</v>
+        <v>7985</v>
       </c>
       <c r="I49" t="n">
         <v>1</v>
@@ -3024,31 +3008,31 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Psoriasis</t>
+          <t>Ovarian polycystic syndrome (PCOS)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Keratinocytes</t>
+          <t>Cortical_organoids_d100</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1.082292018462231</v>
+        <v>0.7489445538981143</v>
       </c>
       <c r="D50" t="n">
-        <v>0.8234780967067024</v>
+        <v>0.7721074750517859</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F50" t="n">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="G50" t="n">
-        <v>846</v>
+        <v>2907</v>
       </c>
       <c r="H50" t="n">
-        <v>9614</v>
+        <v>7983</v>
       </c>
       <c r="I50" t="n">
         <v>1</v>
@@ -3068,31 +3052,31 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Colon diverticulosis</t>
+          <t>Bronchial asthma</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Pooled_epidermis</t>
+          <t>Skeletal_myocyte_(SKM)</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.985393658710367</v>
+        <v>0.9583581507957776</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>0.7933947164465431</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="F51" t="n">
-        <v>49</v>
+        <v>289</v>
       </c>
       <c r="G51" t="n">
-        <v>401</v>
+        <v>2957</v>
       </c>
       <c r="H51" t="n">
-        <v>9681</v>
+        <v>11219</v>
       </c>
       <c r="I51" t="n">
         <v>1</v>
@@ -3100,43 +3084,59 @@
       <c r="J51" t="b">
         <v>0</v>
       </c>
-      <c r="K51" t="inlineStr"/>
-      <c r="L51" t="inlineStr"/>
-      <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr"/>
-      <c r="O51" t="inlineStr"/>
-      <c r="P51" t="inlineStr"/>
-      <c r="Q51" t="inlineStr"/>
-      <c r="R51" t="inlineStr"/>
+      <c r="K51" t="n">
+        <v>1.096785471496552</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0.723448293904273</v>
+      </c>
+      <c r="M51" t="n">
+        <v>38</v>
+      </c>
+      <c r="N51" t="n">
+        <v>35</v>
+      </c>
+      <c r="O51" t="n">
+        <v>1471</v>
+      </c>
+      <c r="P51" t="n">
+        <v>1486</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>0.9503205265004374</v>
+      </c>
+      <c r="R51" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Acne vulgaris</t>
+          <t>aneurysm</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>HF_Sebocytes</t>
+          <t>Pooled_fibroblasts</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>1.092683467797832</v>
       </c>
       <c r="D52" t="n">
-        <v>1</v>
+        <v>0.7834449794144795</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="G52" t="n">
-        <v>70</v>
+        <v>1093</v>
       </c>
       <c r="H52" t="n">
-        <v>5404</v>
+        <v>9853</v>
       </c>
       <c r="I52" t="n">
         <v>1</v>
@@ -3156,31 +3156,31 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Scoliosis</t>
+          <t>Osteoarthritis</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>9_Chondrocytes</t>
+          <t>8_Also_Prechondral_Mesenchyme</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.6099667774086379</v>
+        <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>0.7730263349053912</v>
+        <v>1</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>215</v>
+        <v>50</v>
       </c>
       <c r="G53" t="n">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="H53" t="n">
-        <v>6885</v>
+        <v>6948</v>
       </c>
       <c r="I53" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
added plots and Mann-whitney analysis
</commit_message>
<xml_diff>
--- a/fisher_for_all_data.xlsx
+++ b/fisher_for_all_data.xlsx
@@ -588,31 +588,31 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Alzheimer's Disease</t>
+          <t>Scoliosis</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cortical_organoids_d100</t>
+          <t>CNCCs</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.6683710831609646</v>
+        <v>1.608940531763751</v>
       </c>
       <c r="D3" t="n">
-        <v>2.195838542923922e-05</v>
+        <v>1.989960515490272e-05</v>
       </c>
       <c r="E3" t="n">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="F3" t="n">
-        <v>562</v>
+        <v>208</v>
       </c>
       <c r="G3" t="n">
-        <v>2770</v>
+        <v>3411</v>
       </c>
       <c r="H3" t="n">
-        <v>7432</v>
+        <v>7713</v>
       </c>
       <c r="I3" t="n">
         <v>0.000431848246775038</v>
@@ -621,25 +621,25 @@
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>1.12472487160675</v>
+        <v>1.082601054481547</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5444108617705408</v>
+        <v>0.6749014804308221</v>
       </c>
       <c r="M3" t="n">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="N3" t="n">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="O3" t="n">
-        <v>1363</v>
+        <v>1707</v>
       </c>
       <c r="P3" t="n">
-        <v>1407</v>
+        <v>1704</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.9221139444327839</v>
+        <v>0.9408173212354329</v>
       </c>
       <c r="R3" t="b">
         <v>0</v>
@@ -648,31 +648,31 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Scoliosis</t>
+          <t>Alzheimer's Disease</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CNCCs</t>
+          <t>Cortical_organoids_d100</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.608940531763751</v>
+        <v>0.6683710831609646</v>
       </c>
       <c r="D4" t="n">
-        <v>1.989960515490272e-05</v>
+        <v>2.195838542923922e-05</v>
       </c>
       <c r="E4" t="n">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="F4" t="n">
-        <v>208</v>
+        <v>562</v>
       </c>
       <c r="G4" t="n">
-        <v>3411</v>
+        <v>2770</v>
       </c>
       <c r="H4" t="n">
-        <v>7713</v>
+        <v>7432</v>
       </c>
       <c r="I4" t="n">
         <v>0.000431848246775038</v>
@@ -681,25 +681,25 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>1.082601054481547</v>
+        <v>1.12472487160675</v>
       </c>
       <c r="L4" t="n">
-        <v>0.6749014804308221</v>
+        <v>0.5444108617705408</v>
       </c>
       <c r="M4" t="n">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="N4" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="O4" t="n">
-        <v>1707</v>
+        <v>1363</v>
       </c>
       <c r="P4" t="n">
-        <v>1704</v>
+        <v>1407</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.9408173212354329</v>
+        <v>0.9221139444327839</v>
       </c>
       <c r="R4" t="b">
         <v>0</v>
@@ -1068,31 +1068,31 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Back Disorders</t>
+          <t>Ovarian polycystic syndrome (PCOS)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4_Prechondral_Mesenchyme</t>
+          <t>Cortical_organoids_d50</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.1773528847996933</v>
       </c>
       <c r="D11" t="n">
-        <v>0.07907646134494326</v>
+        <v>0.07437721465595361</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="G11" t="n">
-        <v>386</v>
+        <v>3478</v>
       </c>
       <c r="H11" t="n">
-        <v>9300</v>
+        <v>7402</v>
       </c>
       <c r="I11" t="n">
         <v>0.3883549313822752</v>
@@ -1112,31 +1112,31 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ovarian polycystic syndrome (PCOS)</t>
+          <t>Alzheimer's Disease</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Cortical_organoids_d50</t>
+          <t>Cortical_organoids_d150</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.1773528847996933</v>
+        <v>0.8544395223420647</v>
       </c>
       <c r="D12" t="n">
-        <v>0.07437721465595361</v>
+        <v>0.08556973064355217</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="F12" t="n">
-        <v>12</v>
+        <v>528</v>
       </c>
       <c r="G12" t="n">
-        <v>3478</v>
+        <v>2714</v>
       </c>
       <c r="H12" t="n">
-        <v>7402</v>
+        <v>7245</v>
       </c>
       <c r="I12" t="n">
         <v>0.3883549313822752</v>
@@ -1144,14 +1144,30 @@
       <c r="J12" t="b">
         <v>0</v>
       </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
+      <c r="K12" t="n">
+        <v>1.052989616899391</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.7517813221899442</v>
+      </c>
+      <c r="M12" t="n">
+        <v>85</v>
+      </c>
+      <c r="N12" t="n">
+        <v>84</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1330</v>
+      </c>
+      <c r="P12" t="n">
+        <v>1384</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.9408173212354329</v>
+      </c>
+      <c r="R12" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1216,31 +1232,31 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Alzheimer's Disease</t>
+          <t>Back Disorders</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Cortical_organoids_d150</t>
+          <t>4_Prechondral_Mesenchyme</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.8544395223420647</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.08556973064355217</v>
+        <v>0.07907646134494326</v>
       </c>
       <c r="E14" t="n">
-        <v>169</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>528</v>
+        <v>82</v>
       </c>
       <c r="G14" t="n">
-        <v>2714</v>
+        <v>386</v>
       </c>
       <c r="H14" t="n">
-        <v>7245</v>
+        <v>9300</v>
       </c>
       <c r="I14" t="n">
         <v>0.3883549313822752</v>
@@ -1248,30 +1264,14 @@
       <c r="J14" t="b">
         <v>0</v>
       </c>
-      <c r="K14" t="n">
-        <v>1.052989616899391</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0.7517813221899442</v>
-      </c>
-      <c r="M14" t="n">
-        <v>85</v>
-      </c>
-      <c r="N14" t="n">
-        <v>84</v>
-      </c>
-      <c r="O14" t="n">
-        <v>1330</v>
-      </c>
-      <c r="P14" t="n">
-        <v>1384</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>0.9408173212354329</v>
-      </c>
-      <c r="R14" t="b">
-        <v>0</v>
-      </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1336,31 +1336,31 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Muscular dystrophy</t>
+          <t>carcinoma</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Skeletal_myocyte_(SKM)</t>
+          <t>Pancreatic_progenitor_(PP)</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.5499887881602973</v>
+        <v>1.108819359601728</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1061957063384298</v>
+        <v>0.1110302720267702</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>471</v>
       </c>
       <c r="F16" t="n">
-        <v>62</v>
+        <v>569</v>
       </c>
       <c r="G16" t="n">
-        <v>3021</v>
+        <v>5649</v>
       </c>
       <c r="H16" t="n">
-        <v>11446</v>
+        <v>7567</v>
       </c>
       <c r="I16" t="n">
         <v>0.4094241280987149</v>
@@ -1368,43 +1368,59 @@
       <c r="J16" t="b">
         <v>0</v>
       </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
+      <c r="K16" t="n">
+        <v>0.9876987447698745</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.9236011123687078</v>
+      </c>
+      <c r="M16" t="n">
+        <v>232</v>
+      </c>
+      <c r="N16" t="n">
+        <v>239</v>
+      </c>
+      <c r="O16" t="n">
+        <v>2800</v>
+      </c>
+      <c r="P16" t="n">
+        <v>2849</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.9591242320751966</v>
+      </c>
+      <c r="R16" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>carcinoma</t>
+          <t>Muscular dystrophy</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Pancreatic_progenitor_(PP)</t>
+          <t>Skeletal_myocyte_(SKM)</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1.108819359601728</v>
+        <v>0.5499887881602973</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1110302720267702</v>
+        <v>0.1061957063384298</v>
       </c>
       <c r="E17" t="n">
-        <v>471</v>
+        <v>9</v>
       </c>
       <c r="F17" t="n">
-        <v>569</v>
+        <v>62</v>
       </c>
       <c r="G17" t="n">
-        <v>5649</v>
+        <v>3021</v>
       </c>
       <c r="H17" t="n">
-        <v>7567</v>
+        <v>11446</v>
       </c>
       <c r="I17" t="n">
         <v>0.4094241280987149</v>
@@ -1412,30 +1428,14 @@
       <c r="J17" t="b">
         <v>0</v>
       </c>
-      <c r="K17" t="n">
-        <v>0.9876987447698745</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0.9236011123687078</v>
-      </c>
-      <c r="M17" t="n">
-        <v>232</v>
-      </c>
-      <c r="N17" t="n">
-        <v>239</v>
-      </c>
-      <c r="O17" t="n">
-        <v>2800</v>
-      </c>
-      <c r="P17" t="n">
-        <v>2849</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>0.9591242320751966</v>
-      </c>
-      <c r="R17" t="b">
-        <v>0</v>
-      </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1500,31 +1500,31 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Bipolar disorder</t>
+          <t>Colon diverticulosis</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Cortical_organoids_d100</t>
+          <t>Skeletal_myocyte_(SKM)</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.8306901905434015</v>
+        <v>1.463838487094301</v>
       </c>
       <c r="D19" t="n">
-        <v>0.181724572324664</v>
+        <v>0.1470466708278776</v>
       </c>
       <c r="E19" t="n">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="F19" t="n">
-        <v>250</v>
+        <v>52</v>
       </c>
       <c r="G19" t="n">
-        <v>2834</v>
+        <v>3010</v>
       </c>
       <c r="H19" t="n">
-        <v>7744</v>
+        <v>11456</v>
       </c>
       <c r="I19" t="n">
         <v>0.4467395736314655</v>
@@ -1533,25 +1533,25 @@
         <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>0.6257920125814695</v>
+        <v>0.8236363636363636</v>
       </c>
       <c r="L19" t="n">
-        <v>0.04894373111450499</v>
+        <v>0.8232465332793673</v>
       </c>
       <c r="M19" t="n">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="N19" t="n">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="O19" t="n">
-        <v>1407</v>
+        <v>1500</v>
       </c>
       <c r="P19" t="n">
-        <v>1427</v>
+        <v>1510</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.2870649952337803</v>
+        <v>0.9408173212354329</v>
       </c>
       <c r="R19" t="b">
         <v>0</v>
@@ -1560,31 +1560,31 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Colon diverticulosis</t>
+          <t>Bipolar disorder</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Skeletal_myocyte_(SKM)</t>
+          <t>Cortical_organoids_d100</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1.463838487094301</v>
+        <v>0.8306901905434015</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1470466708278776</v>
+        <v>0.181724572324664</v>
       </c>
       <c r="E20" t="n">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F20" t="n">
-        <v>52</v>
+        <v>250</v>
       </c>
       <c r="G20" t="n">
-        <v>3010</v>
+        <v>2834</v>
       </c>
       <c r="H20" t="n">
-        <v>11456</v>
+        <v>7744</v>
       </c>
       <c r="I20" t="n">
         <v>0.4467395736314655</v>
@@ -1593,25 +1593,25 @@
         <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>0.8236363636363636</v>
+        <v>0.6257920125814695</v>
       </c>
       <c r="L20" t="n">
-        <v>0.8232465332793673</v>
+        <v>0.04894373111450499</v>
       </c>
       <c r="M20" t="n">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="N20" t="n">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="O20" t="n">
-        <v>1500</v>
+        <v>1407</v>
       </c>
       <c r="P20" t="n">
-        <v>1510</v>
+        <v>1427</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.9408173212354329</v>
+        <v>0.2870649952337803</v>
       </c>
       <c r="R20" t="b">
         <v>0</v>
@@ -1620,31 +1620,31 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Varicose veins</t>
+          <t>carcinoma</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Endothelial_not_treated</t>
+          <t>Pooled_epidermis</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.3048483598101919</v>
+        <v>0.7342389374245329</v>
       </c>
       <c r="D21" t="n">
-        <v>0.1416314841859758</v>
+        <v>0.1771624268749524</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="F21" t="n">
-        <v>10</v>
+        <v>741</v>
       </c>
       <c r="G21" t="n">
-        <v>4847</v>
+        <v>380</v>
       </c>
       <c r="H21" t="n">
-        <v>7388</v>
+        <v>8989</v>
       </c>
       <c r="I21" t="n">
         <v>0.4467395736314655</v>
@@ -1652,43 +1652,59 @@
       <c r="J21" t="b">
         <v>0</v>
       </c>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr"/>
+      <c r="K21" t="n">
+        <v>2.486656200941915</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.0531601843025519</v>
+      </c>
+      <c r="M21" t="n">
+        <v>16</v>
+      </c>
+      <c r="N21" t="n">
+        <v>7</v>
+      </c>
+      <c r="O21" t="n">
+        <v>182</v>
+      </c>
+      <c r="P21" t="n">
+        <v>198</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.2870649952337803</v>
+      </c>
+      <c r="R21" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>carcinoma</t>
+          <t>Osteoarthritis</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Pooled_epidermis</t>
+          <t>4_Prechondral_Mesenchyme</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.7342389374245329</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1771624268749524</v>
+        <v>0.1759116570297418</v>
       </c>
       <c r="E22" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>741</v>
+        <v>60</v>
       </c>
       <c r="G22" t="n">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="H22" t="n">
-        <v>8989</v>
+        <v>9322</v>
       </c>
       <c r="I22" t="n">
         <v>0.4467395736314655</v>
@@ -1696,30 +1712,14 @@
       <c r="J22" t="b">
         <v>0</v>
       </c>
-      <c r="K22" t="n">
-        <v>2.486656200941915</v>
-      </c>
-      <c r="L22" t="n">
-        <v>0.0531601843025519</v>
-      </c>
-      <c r="M22" t="n">
-        <v>16</v>
-      </c>
-      <c r="N22" t="n">
-        <v>7</v>
-      </c>
-      <c r="O22" t="n">
-        <v>182</v>
-      </c>
-      <c r="P22" t="n">
-        <v>198</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>0.2870649952337803</v>
-      </c>
-      <c r="R22" t="b">
-        <v>0</v>
-      </c>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1828,31 +1828,31 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Osteoarthritis</t>
+          <t>Varicose veins</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4_Prechondral_Mesenchyme</t>
+          <t>Endothelial_not_treated</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>0.3048483598101919</v>
       </c>
       <c r="D25" t="n">
-        <v>0.1759116570297418</v>
+        <v>0.1416314841859758</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="G25" t="n">
-        <v>386</v>
+        <v>4847</v>
       </c>
       <c r="H25" t="n">
-        <v>9322</v>
+        <v>7388</v>
       </c>
       <c r="I25" t="n">
         <v>0.4467395736314655</v>
@@ -2168,31 +2168,31 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Ovarian polycystic syndrome (PCOS)</t>
+          <t>Alzheimer's Disease</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Skeletal_myocyte_(SKM)</t>
+          <t>Cortical_organoids_d50</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.4744055482166447</v>
+        <v>0.9302362362864961</v>
       </c>
       <c r="D32" t="n">
-        <v>0.3974935686153851</v>
+        <v>0.4029007018739673</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>214</v>
       </c>
       <c r="F32" t="n">
-        <v>16</v>
+        <v>488</v>
       </c>
       <c r="G32" t="n">
-        <v>3028</v>
+        <v>3265</v>
       </c>
       <c r="H32" t="n">
-        <v>11492</v>
+        <v>6926</v>
       </c>
       <c r="I32" t="n">
         <v>0.7428481690801272</v>
@@ -2200,43 +2200,59 @@
       <c r="J32" t="b">
         <v>0</v>
       </c>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
-      <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr"/>
+      <c r="K32" t="n">
+        <v>1.088241620362072</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.5726477153681263</v>
+      </c>
+      <c r="M32" t="n">
+        <v>109</v>
+      </c>
+      <c r="N32" t="n">
+        <v>105</v>
+      </c>
+      <c r="O32" t="n">
+        <v>1594</v>
+      </c>
+      <c r="P32" t="n">
+        <v>1671</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.9221139444327839</v>
+      </c>
+      <c r="R32" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Alzheimer's Disease</t>
+          <t>Ovarian polycystic syndrome (PCOS)</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Cortical_organoids_d50</t>
+          <t>Skeletal_myocyte_(SKM)</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.9302362362864961</v>
+        <v>0.4744055482166447</v>
       </c>
       <c r="D33" t="n">
-        <v>0.4029007018739673</v>
+        <v>0.3974935686153851</v>
       </c>
       <c r="E33" t="n">
-        <v>214</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
-        <v>488</v>
+        <v>16</v>
       </c>
       <c r="G33" t="n">
-        <v>3265</v>
+        <v>3028</v>
       </c>
       <c r="H33" t="n">
-        <v>6926</v>
+        <v>11492</v>
       </c>
       <c r="I33" t="n">
         <v>0.7428481690801272</v>
@@ -2244,59 +2260,43 @@
       <c r="J33" t="b">
         <v>0</v>
       </c>
-      <c r="K33" t="n">
-        <v>1.088241620362072</v>
-      </c>
-      <c r="L33" t="n">
-        <v>0.5726477153681263</v>
-      </c>
-      <c r="M33" t="n">
-        <v>109</v>
-      </c>
-      <c r="N33" t="n">
-        <v>105</v>
-      </c>
-      <c r="O33" t="n">
-        <v>1594</v>
-      </c>
-      <c r="P33" t="n">
-        <v>1671</v>
-      </c>
-      <c r="Q33" t="n">
-        <v>0.9221139444327839</v>
-      </c>
-      <c r="R33" t="b">
-        <v>0</v>
-      </c>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Osteoarthritis</t>
+          <t>Scoliosis</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>9_Chondrocytes</t>
+          <t>Skeletal_myocyte_(SKM)</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1.585354896675651</v>
+        <v>0.9116883268459783</v>
       </c>
       <c r="D34" t="n">
-        <v>0.4753843662171084</v>
+        <v>0.4717008145713483</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="F34" t="n">
-        <v>42</v>
+        <v>349</v>
       </c>
       <c r="G34" t="n">
-        <v>106</v>
+        <v>2946</v>
       </c>
       <c r="H34" t="n">
-        <v>7058</v>
+        <v>11159</v>
       </c>
       <c r="I34" t="n">
         <v>0.8249316943179235</v>
@@ -2304,43 +2304,59 @@
       <c r="J34" t="b">
         <v>0</v>
       </c>
-      <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
-      <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="inlineStr"/>
+      <c r="K34" t="n">
+        <v>0.8702040816326531</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.5805902613095306</v>
+      </c>
+      <c r="M34" t="n">
+        <v>39</v>
+      </c>
+      <c r="N34" t="n">
+        <v>45</v>
+      </c>
+      <c r="O34" t="n">
+        <v>1470</v>
+      </c>
+      <c r="P34" t="n">
+        <v>1476</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0.9221139444327839</v>
+      </c>
+      <c r="R34" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Scoliosis</t>
+          <t>Osteoarthritis</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Skeletal_myocyte_(SKM)</t>
+          <t>9_Chondrocytes</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.9116883268459783</v>
+        <v>1.585354896675651</v>
       </c>
       <c r="D35" t="n">
-        <v>0.4717008145713483</v>
+        <v>0.4753843662171084</v>
       </c>
       <c r="E35" t="n">
-        <v>84</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
-        <v>349</v>
+        <v>42</v>
       </c>
       <c r="G35" t="n">
-        <v>2946</v>
+        <v>106</v>
       </c>
       <c r="H35" t="n">
-        <v>11159</v>
+        <v>7058</v>
       </c>
       <c r="I35" t="n">
         <v>0.8249316943179235</v>
@@ -2348,30 +2364,14 @@
       <c r="J35" t="b">
         <v>0</v>
       </c>
-      <c r="K35" t="n">
-        <v>0.8702040816326531</v>
-      </c>
-      <c r="L35" t="n">
-        <v>0.5805902613095306</v>
-      </c>
-      <c r="M35" t="n">
-        <v>39</v>
-      </c>
-      <c r="N35" t="n">
-        <v>45</v>
-      </c>
-      <c r="O35" t="n">
-        <v>1470</v>
-      </c>
-      <c r="P35" t="n">
-        <v>1476</v>
-      </c>
-      <c r="Q35" t="n">
-        <v>0.9221139444327839</v>
-      </c>
-      <c r="R35" t="b">
-        <v>0</v>
-      </c>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr"/>
+      <c r="R35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2732,31 +2732,31 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Colon diverticulosis</t>
+          <t>Osteoarthritis</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Pooled_epidermis</t>
+          <t>8_Also_Prechondral_Mesenchyme</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.985393658710367</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
         <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G43" t="n">
-        <v>401</v>
+        <v>76</v>
       </c>
       <c r="H43" t="n">
-        <v>9681</v>
+        <v>6948</v>
       </c>
       <c r="I43" t="n">
         <v>1</v>
@@ -2776,31 +2776,31 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Sleep apnea</t>
+          <t>Acne vulgaris</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Cortical_organoids_d100</t>
+          <t>Keratinocytes</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.9156060084852654</v>
+        <v>1.032620320855615</v>
       </c>
       <c r="D44" t="n">
         <v>1</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G44" t="n">
-        <v>2907</v>
+        <v>850</v>
       </c>
       <c r="H44" t="n">
-        <v>7985</v>
+        <v>9655</v>
       </c>
       <c r="I44" t="n">
         <v>1</v>
@@ -2825,26 +2825,26 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>HF_Sebocytes</t>
+          <t>Pooled_fibroblasts</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>0.8580126114372689</v>
       </c>
       <c r="D45" t="n">
         <v>1</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G45" t="n">
-        <v>70</v>
+        <v>1095</v>
       </c>
       <c r="H45" t="n">
-        <v>5404</v>
+        <v>9865</v>
       </c>
       <c r="I45" t="n">
         <v>1</v>
@@ -2864,31 +2864,31 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Sleep apnea</t>
+          <t>Ovarian polycystic syndrome (PCOS)</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Cortical_organoids_d50</t>
+          <t>Cortical_organoids_d100</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.7101074031453778</v>
+        <v>0.7489445538981143</v>
       </c>
       <c r="D46" t="n">
-        <v>0.7626901108875515</v>
+        <v>0.7721074750517859</v>
       </c>
       <c r="E46" t="n">
         <v>3</v>
       </c>
       <c r="F46" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G46" t="n">
-        <v>3476</v>
+        <v>2907</v>
       </c>
       <c r="H46" t="n">
-        <v>7405</v>
+        <v>7983</v>
       </c>
       <c r="I46" t="n">
         <v>1</v>
@@ -2908,31 +2908,31 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Sleep apnea</t>
+          <t>aneurysm</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Skeletal_myocyte_(SKM)</t>
+          <t>Pooled_fibroblasts</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.9494549058473737</v>
+        <v>1.092683467797832</v>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>0.7834449794144795</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="G47" t="n">
-        <v>3027</v>
+        <v>1093</v>
       </c>
       <c r="H47" t="n">
-        <v>11496</v>
+        <v>9853</v>
       </c>
       <c r="I47" t="n">
         <v>1</v>
@@ -2952,31 +2952,31 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Sleep apnea</t>
+          <t>Bronchial asthma</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Cortical_organoids_d150</t>
+          <t>Skeletal_myocyte_(SKM)</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.8086458333333333</v>
+        <v>0.9583581507957776</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>0.7933947164465431</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="F48" t="n">
-        <v>10</v>
+        <v>289</v>
       </c>
       <c r="G48" t="n">
-        <v>2880</v>
+        <v>2957</v>
       </c>
       <c r="H48" t="n">
-        <v>7763</v>
+        <v>11219</v>
       </c>
       <c r="I48" t="n">
         <v>1</v>
@@ -2984,28 +2984,44 @@
       <c r="J48" t="b">
         <v>0</v>
       </c>
-      <c r="K48" t="inlineStr"/>
-      <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
-      <c r="O48" t="inlineStr"/>
-      <c r="P48" t="inlineStr"/>
-      <c r="Q48" t="inlineStr"/>
-      <c r="R48" t="inlineStr"/>
+      <c r="K48" t="n">
+        <v>1.096785471496552</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0.723448293904273</v>
+      </c>
+      <c r="M48" t="n">
+        <v>38</v>
+      </c>
+      <c r="N48" t="n">
+        <v>35</v>
+      </c>
+      <c r="O48" t="n">
+        <v>1471</v>
+      </c>
+      <c r="P48" t="n">
+        <v>1486</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>0.9408173212354329</v>
+      </c>
+      <c r="R48" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Acne vulgaris</t>
+          <t>Colon diverticulosis</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Pooled_fibroblasts</t>
+          <t>Pooled_epidermis</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.8580126114372689</v>
+        <v>0.985393658710367</v>
       </c>
       <c r="D49" t="n">
         <v>1</v>
@@ -3014,13 +3030,13 @@
         <v>2</v>
       </c>
       <c r="F49" t="n">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="G49" t="n">
-        <v>1095</v>
+        <v>401</v>
       </c>
       <c r="H49" t="n">
-        <v>9865</v>
+        <v>9681</v>
       </c>
       <c r="I49" t="n">
         <v>1</v>
@@ -3040,31 +3056,31 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>carcinoma</t>
+          <t>Scoliosis</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Hepatocyte_Progenitor_(HP)</t>
+          <t>9_Chondrocytes</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.9987109652706972</v>
+        <v>0.6099667774086379</v>
       </c>
       <c r="D50" t="n">
-        <v>1</v>
+        <v>0.7730263349053912</v>
       </c>
       <c r="E50" t="n">
-        <v>438</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
-        <v>568</v>
+        <v>215</v>
       </c>
       <c r="G50" t="n">
-        <v>5567</v>
+        <v>105</v>
       </c>
       <c r="H50" t="n">
-        <v>7210</v>
+        <v>6885</v>
       </c>
       <c r="I50" t="n">
         <v>1</v>
@@ -3072,59 +3088,43 @@
       <c r="J50" t="b">
         <v>0</v>
       </c>
-      <c r="K50" t="n">
-        <v>1.073898606097515</v>
-      </c>
-      <c r="L50" t="n">
-        <v>0.4873909825454742</v>
-      </c>
-      <c r="M50" t="n">
-        <v>227</v>
-      </c>
-      <c r="N50" t="n">
-        <v>211</v>
-      </c>
-      <c r="O50" t="n">
-        <v>2786</v>
-      </c>
-      <c r="P50" t="n">
-        <v>2781</v>
-      </c>
-      <c r="Q50" t="n">
-        <v>0.9221139444327839</v>
-      </c>
-      <c r="R50" t="b">
-        <v>0</v>
-      </c>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+      <c r="Q50" t="inlineStr"/>
+      <c r="R50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Back Disorders</t>
+          <t>Psoriasis</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>8_Also_Prechondral_Mesenchyme</t>
+          <t>Keratinocytes</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>1.082292018462231</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>0.8234780967067024</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="G51" t="n">
-        <v>76</v>
+        <v>846</v>
       </c>
       <c r="H51" t="n">
-        <v>6945</v>
+        <v>9614</v>
       </c>
       <c r="I51" t="n">
         <v>1</v>
@@ -3144,31 +3144,31 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Acne vulgaris</t>
+          <t>Osteoporosis</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Keratinocytes</t>
+          <t>9_Chondrocytes</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1.032620320855615</v>
+        <v>0</v>
       </c>
       <c r="D52" t="n">
         <v>1</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="G52" t="n">
-        <v>850</v>
+        <v>107</v>
       </c>
       <c r="H52" t="n">
-        <v>9655</v>
+        <v>7089</v>
       </c>
       <c r="I52" t="n">
         <v>1</v>
@@ -3188,31 +3188,31 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Psoriasis</t>
+          <t>Sleep apnea</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Keratinocytes</t>
+          <t>Skeletal_myocyte_(SKM)</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1.082292018462231</v>
+        <v>0.9494549058473737</v>
       </c>
       <c r="D53" t="n">
-        <v>0.8234780967067024</v>
+        <v>1</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="G53" t="n">
-        <v>846</v>
+        <v>3027</v>
       </c>
       <c r="H53" t="n">
-        <v>9614</v>
+        <v>11496</v>
       </c>
       <c r="I53" t="n">
         <v>1</v>
@@ -3232,31 +3232,31 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>aneurysm</t>
+          <t>carcinoma</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Pooled_fibroblasts</t>
+          <t>Hepatocyte_Progenitor_(HP)</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1.092683467797832</v>
+        <v>0.9987109652706972</v>
       </c>
       <c r="D54" t="n">
-        <v>0.7834449794144795</v>
+        <v>1</v>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>438</v>
       </c>
       <c r="F54" t="n">
-        <v>33</v>
+        <v>568</v>
       </c>
       <c r="G54" t="n">
-        <v>1093</v>
+        <v>5567</v>
       </c>
       <c r="H54" t="n">
-        <v>9853</v>
+        <v>7210</v>
       </c>
       <c r="I54" t="n">
         <v>1</v>
@@ -3264,43 +3264,59 @@
       <c r="J54" t="b">
         <v>0</v>
       </c>
-      <c r="K54" t="inlineStr"/>
-      <c r="L54" t="inlineStr"/>
-      <c r="M54" t="inlineStr"/>
-      <c r="N54" t="inlineStr"/>
-      <c r="O54" t="inlineStr"/>
-      <c r="P54" t="inlineStr"/>
-      <c r="Q54" t="inlineStr"/>
-      <c r="R54" t="inlineStr"/>
+      <c r="K54" t="n">
+        <v>1.073898606097515</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0.4873909825454742</v>
+      </c>
+      <c r="M54" t="n">
+        <v>227</v>
+      </c>
+      <c r="N54" t="n">
+        <v>211</v>
+      </c>
+      <c r="O54" t="n">
+        <v>2786</v>
+      </c>
+      <c r="P54" t="n">
+        <v>2781</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>0.9221139444327839</v>
+      </c>
+      <c r="R54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Scoliosis</t>
+          <t>Sleep apnea</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>9_Chondrocytes</t>
+          <t>Cortical_organoids_d50</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.6099667774086379</v>
+        <v>0.7101074031453778</v>
       </c>
       <c r="D55" t="n">
-        <v>0.7730263349053912</v>
+        <v>0.7626901108875515</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
-        <v>215</v>
+        <v>9</v>
       </c>
       <c r="G55" t="n">
-        <v>105</v>
+        <v>3476</v>
       </c>
       <c r="H55" t="n">
-        <v>6885</v>
+        <v>7405</v>
       </c>
       <c r="I55" t="n">
         <v>1</v>
@@ -3320,31 +3336,31 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Bronchial asthma</t>
+          <t>Sleep apnea</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Skeletal_myocyte_(SKM)</t>
+          <t>Cortical_organoids_d100</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.9583581507957776</v>
+        <v>0.9156060084852654</v>
       </c>
       <c r="D56" t="n">
-        <v>0.7933947164465431</v>
+        <v>1</v>
       </c>
       <c r="E56" t="n">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="F56" t="n">
-        <v>289</v>
+        <v>9</v>
       </c>
       <c r="G56" t="n">
-        <v>2957</v>
+        <v>2907</v>
       </c>
       <c r="H56" t="n">
-        <v>11219</v>
+        <v>7985</v>
       </c>
       <c r="I56" t="n">
         <v>1</v>
@@ -3352,59 +3368,43 @@
       <c r="J56" t="b">
         <v>0</v>
       </c>
-      <c r="K56" t="n">
-        <v>1.096785471496552</v>
-      </c>
-      <c r="L56" t="n">
-        <v>0.723448293904273</v>
-      </c>
-      <c r="M56" t="n">
-        <v>38</v>
-      </c>
-      <c r="N56" t="n">
-        <v>35</v>
-      </c>
-      <c r="O56" t="n">
-        <v>1471</v>
-      </c>
-      <c r="P56" t="n">
-        <v>1486</v>
-      </c>
-      <c r="Q56" t="n">
-        <v>0.9408173212354329</v>
-      </c>
-      <c r="R56" t="b">
-        <v>0</v>
-      </c>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
+      <c r="R56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Ovarian polycystic syndrome (PCOS)</t>
+          <t>Sleep apnea</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Cortical_organoids_d100</t>
+          <t>Cortical_organoids_d150</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.7489445538981143</v>
+        <v>0.8086458333333333</v>
       </c>
       <c r="D57" t="n">
-        <v>0.7721074750517859</v>
+        <v>1</v>
       </c>
       <c r="E57" t="n">
         <v>3</v>
       </c>
       <c r="F57" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G57" t="n">
-        <v>2907</v>
+        <v>2880</v>
       </c>
       <c r="H57" t="n">
-        <v>7983</v>
+        <v>7763</v>
       </c>
       <c r="I57" t="n">
         <v>1</v>
@@ -3424,7 +3424,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Osteoarthritis</t>
+          <t>Back Disorders</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -3442,13 +3442,13 @@
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G58" t="n">
         <v>76</v>
       </c>
       <c r="H58" t="n">
-        <v>6948</v>
+        <v>6945</v>
       </c>
       <c r="I58" t="n">
         <v>1</v>
@@ -3468,12 +3468,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Osteoporosis</t>
+          <t>Acne vulgaris</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>9_Chondrocytes</t>
+          <t>HF_Sebocytes</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -3486,13 +3486,13 @@
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G59" t="n">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="H59" t="n">
-        <v>7089</v>
+        <v>5404</v>
       </c>
       <c r="I59" t="n">
         <v>1</v>

</xml_diff>